<commit_message>
add default group to mobile
</commit_message>
<xml_diff>
--- a/src/assets/smslo.schema.mobiles.xlsx
+++ b/src/assets/smslo.schema.mobiles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\smsli\src\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AC37DA0-707C-4698-9B6B-4B389BA402EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34B9AEA2-4CDC-44E4-ACF4-CEA562DF4715}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1290" yWindow="-110" windowWidth="18020" windowHeight="11020" xr2:uid="{8FCD3274-18F1-4FF0-85D7-131854D0C1ED}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>שם פרטי</t>
   </si>
@@ -44,15 +44,57 @@
     <t>סלולרי</t>
   </si>
   <si>
-    <t>קבוצה</t>
+    <t>אברהם</t>
+  </si>
+  <si>
+    <t>אברהמי</t>
+  </si>
+  <si>
+    <t>052-1234567</t>
+  </si>
+  <si>
+    <t>בעלי עסקים</t>
+  </si>
+  <si>
+    <t>כללי</t>
+  </si>
+  <si>
+    <t>יעקב</t>
+  </si>
+  <si>
+    <t>יעקובי</t>
+  </si>
+  <si>
+    <t>יצחק</t>
+  </si>
+  <si>
+    <t>יצחקי</t>
+  </si>
+  <si>
+    <t>פריימריז</t>
+  </si>
+  <si>
+    <t>קבוצה ראשית</t>
+  </si>
+  <si>
+    <t>055-1234-567</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -80,8 +122,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,38 +444,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FD97B93-FF6B-43A9-9B31-BD47AD023346}">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="9.6328125" customWidth="1"/>
-    <col min="2" max="2" width="12.08984375" customWidth="1"/>
-    <col min="3" max="3" width="11.90625" customWidth="1"/>
+    <col min="1" max="1" width="9.6328125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.08984375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.81640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="11.81640625" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>3</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2">
+        <v>501234567</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{1C3C92C2-4D2C-4247-8603-51FB0DC60F1D}">
-      <formula1>"בעלי עסקים,ליכוד,פריימריז,קמפיין לבחירות ביבי"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D1048576" xr:uid="{8055DE88-5423-4526-9EC1-313A7D62E4DB}">
+      <formula1>"בעלי עסקים,ליכוד,פריימריז,קמפיין לבחירות ביבי,כללי"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>